<commit_message>
Transp Fixes to Aircraft
</commit_message>
<xml_diff>
--- a/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
+++ b/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\Brazil\Model\InputData\trans\SYFAFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4D52E2-6B8E-48CE-98ED-26883ABC1BC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3BB4D7-7965-4C89-B351-1C12B753439F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41055" yWindow="1005" windowWidth="25725" windowHeight="9030" tabRatio="742" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40305" yWindow="1740" windowWidth="25200" windowHeight="11640" tabRatio="742" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="ti_tbl_69" localSheetId="5">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -527,7 +527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,6 +676,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1148,7 +1160,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1177,10 +1189,14 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="42" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="41" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="42" fillId="28" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="41" fillId="28" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="153">
     <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1754,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1864,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1954,6 +1970,9 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="14" spans="1:4">
+      <c r="C14" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1963,8 +1982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BT18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2185,10 +2205,10 @@
       </c>
     </row>
     <row r="2" spans="1:72">
-      <c r="A2" t="s">
+      <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="12"/>
@@ -2215,145 +2235,145 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="15"/>
       <c r="Z2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AA2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AB2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AC2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AD2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AE2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AF2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AG2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AH2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AI2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AJ2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AK2" s="14">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="AL2" s="14">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AM2" s="22">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AN2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AO2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AP2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AQ2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AR2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AS2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AT2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AU2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AV2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AW2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AX2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AY2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="AZ2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BA2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BB2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BC2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BD2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BE2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BF2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BG2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BH2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BI2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BJ2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BK2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BL2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BM2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BN2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BO2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BP2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BQ2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BR2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BS2" s="23">
-        <v>3.8531369427586355E-4</v>
-      </c>
-      <c r="BT2" s="23">
-        <v>3.8531369427586355E-4</v>
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AM2" s="24">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AN2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AO2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AP2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AQ2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AR2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AS2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AT2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AU2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AV2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AW2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AX2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AY2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="AZ2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BA2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BB2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BC2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BD2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BE2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BF2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BG2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BH2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BI2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BJ2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BK2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BL2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BM2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BN2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BO2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BP2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BQ2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BR2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BS2" s="22">
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="BT2" s="22">
+        <v>3.8531369427586366E-4</v>
       </c>
     </row>
     <row r="3" spans="1:72">
@@ -2427,114 +2447,114 @@
       <c r="AL3" s="14">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AM3" s="22">
+      <c r="AM3" s="24">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AN3" s="23">
+      <c r="AN3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AO3" s="23">
+      <c r="AO3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AP3" s="23">
+      <c r="AP3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AQ3" s="23">
+      <c r="AQ3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AR3" s="23">
+      <c r="AR3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AS3" s="23">
+      <c r="AS3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AT3" s="23">
+      <c r="AT3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AU3" s="23">
+      <c r="AU3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AV3" s="23">
+      <c r="AV3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AW3" s="23">
+      <c r="AW3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AX3" s="23">
+      <c r="AX3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AY3" s="23">
+      <c r="AY3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="AZ3" s="23">
+      <c r="AZ3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BA3" s="23">
+      <c r="BA3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BB3" s="23">
+      <c r="BB3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BC3" s="23">
+      <c r="BC3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BD3" s="23">
+      <c r="BD3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BE3" s="23">
+      <c r="BE3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BF3" s="23">
+      <c r="BF3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BG3" s="23">
+      <c r="BG3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BH3" s="23">
+      <c r="BH3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BI3" s="23">
+      <c r="BI3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BJ3" s="23">
+      <c r="BJ3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BK3" s="23">
+      <c r="BK3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BL3" s="23">
+      <c r="BL3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BM3" s="23">
+      <c r="BM3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BN3" s="23">
+      <c r="BN3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BO3" s="23">
+      <c r="BO3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BP3" s="23">
+      <c r="BP3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BQ3" s="23">
+      <c r="BQ3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BR3" s="23">
+      <c r="BR3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BS3" s="23">
+      <c r="BS3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="BT3" s="23">
+      <c r="BT3" s="22">
         <v>1.625585658993685E-4</v>
       </c>
     </row>
     <row r="4" spans="1:72">
-      <c r="A4" t="s">
+      <c r="A4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="12"/>
@@ -2619,106 +2639,106 @@
       <c r="AL4" s="14">
         <v>1.7655503230029938E-3</v>
       </c>
-      <c r="AM4" s="22">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AN4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AO4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AP4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AQ4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AR4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AS4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AT4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AU4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AV4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AW4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AX4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AY4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="AZ4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BA4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BB4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BC4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BD4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BE4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BF4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BG4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BH4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BI4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BJ4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BK4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BL4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BM4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BN4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BO4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BP4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BQ4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BR4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BS4" s="23">
-        <v>1.7655503230029938E-3</v>
-      </c>
-      <c r="BT4" s="23">
+      <c r="AM4" s="24">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AN4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AO4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AP4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AQ4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AR4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AS4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AT4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AU4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AV4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AW4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AX4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AY4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="AZ4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BA4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BB4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BC4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BD4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BE4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BF4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BG4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BH4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BI4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BJ4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BK4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BL4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BM4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BN4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BO4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BP4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BQ4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BR4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BS4" s="22">
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="BT4" s="22">
         <v>1.7655503230029938E-3</v>
       </c>
     </row>
@@ -2815,10 +2835,10 @@
       <c r="AJ5" s="14">
         <v>4.7197267347680587E-4</v>
       </c>
-      <c r="AK5" s="24">
+      <c r="AK5" s="23">
         <v>4.7197267347680587E-4</v>
       </c>
-      <c r="AL5" s="24">
+      <c r="AL5" s="23">
         <v>4.7197267347680587E-4</v>
       </c>
       <c r="AM5" s="25">
@@ -2925,10 +2945,10 @@
       </c>
     </row>
     <row r="6" spans="1:72">
-      <c r="A6" t="s">
+      <c r="A6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="12"/>
@@ -2944,178 +2964,178 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="P6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="Q6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="R6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="S6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="T6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="U6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="V6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="W6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="X6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="Y6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="Z6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AA6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AB6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AC6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AD6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AE6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AF6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AG6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AH6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AI6" s="16">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AJ6" s="16">
-        <v>5.3600722376299557E-4</v>
-      </c>
-      <c r="AK6" s="24">
-        <v>5.3600722376299557E-4</v>
-      </c>
-      <c r="AL6" s="24">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
+      </c>
+      <c r="AK6" s="23">
+        <v>6.0343668020558983E-4</v>
+      </c>
+      <c r="AL6" s="23">
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AM6" s="25">
-        <v>5.3600722376299557E-4</v>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="AN6" s="20">
-        <v>5.3614827829556472E-4</v>
+        <v>6.0359547933195961E-4</v>
       </c>
       <c r="AO6" s="20">
-        <v>5.3628936994774769E-4</v>
+        <v>6.0375432024757322E-4</v>
       </c>
       <c r="AP6" s="20">
-        <v>5.364304987293128E-4</v>
+        <v>6.0391320296342783E-4</v>
       </c>
       <c r="AQ6" s="20">
-        <v>5.3657166465003099E-4</v>
+        <v>6.0407212749052344E-4</v>
       </c>
       <c r="AR6" s="20">
-        <v>5.3671286771967569E-4</v>
+        <v>6.0423109383986296E-4</v>
       </c>
       <c r="AS6" s="20">
-        <v>5.3685410794802294E-4</v>
+        <v>6.0439010202245234E-4</v>
       </c>
       <c r="AT6" s="20">
-        <v>5.3699538534485126E-4</v>
+        <v>6.0454915204930025E-4</v>
       </c>
       <c r="AU6" s="20">
-        <v>5.3713669991994201E-4</v>
+        <v>6.0470824393141838E-4</v>
       </c>
       <c r="AV6" s="20">
-        <v>5.372780516830788E-4</v>
+        <v>6.0486737767982137E-4</v>
       </c>
       <c r="AW6" s="20">
-        <v>5.3741944064404797E-4</v>
+        <v>6.0502655330552655E-4</v>
       </c>
       <c r="AX6" s="20">
-        <v>5.3756086681263845E-4</v>
+        <v>6.0518577081955429E-4</v>
       </c>
       <c r="AY6" s="20">
-        <v>5.3770233019864169E-4</v>
+        <v>6.0534503023292779E-4</v>
       </c>
       <c r="AZ6" s="20">
-        <v>5.378438308118518E-4</v>
+        <v>6.0550433155667327E-4</v>
       </c>
       <c r="BA6" s="20">
-        <v>5.3798536866206544E-4</v>
+        <v>6.0566367480181967E-4</v>
       </c>
       <c r="BB6" s="20">
-        <v>5.3812694375908173E-4</v>
+        <v>6.0582305997939907E-4</v>
       </c>
       <c r="BC6" s="20">
-        <v>5.382685561127025E-4</v>
+        <v>6.0598248710044627E-4</v>
       </c>
       <c r="BD6" s="20">
-        <v>5.3841020573273208E-4</v>
+        <v>6.0614195617599898E-4</v>
       </c>
       <c r="BE6" s="20">
-        <v>5.3855189262897753E-4</v>
+        <v>6.0630146721709786E-4</v>
       </c>
       <c r="BF6" s="20">
-        <v>5.3869361681124826E-4</v>
+        <v>6.0646102023478648E-4</v>
       </c>
       <c r="BG6" s="20">
-        <v>5.3883537828935642E-4</v>
+        <v>6.0662061524011134E-4</v>
       </c>
       <c r="BH6" s="20">
-        <v>5.3897717707311675E-4</v>
+        <v>6.0678025224412187E-4</v>
       </c>
       <c r="BI6" s="20">
-        <v>5.3911901317234647E-4</v>
+        <v>6.0693993125787021E-4</v>
       </c>
       <c r="BJ6" s="20">
-        <v>5.3926088659686543E-4</v>
+        <v>6.0709965229241165E-4</v>
       </c>
       <c r="BK6" s="20">
-        <v>5.3940279735649617E-4</v>
+        <v>6.0725941535880428E-4</v>
       </c>
       <c r="BL6" s="20">
-        <v>5.3954474546106363E-4</v>
+        <v>6.0741922046810915E-4</v>
       </c>
       <c r="BM6" s="20">
-        <v>5.3968673092039544E-4</v>
+        <v>6.075790676313902E-4</v>
       </c>
       <c r="BN6" s="20">
-        <v>5.3982875374432185E-4</v>
+        <v>6.0773895685971421E-4</v>
       </c>
       <c r="BO6" s="20">
-        <v>5.399708139426756E-4</v>
+        <v>6.0789888816415089E-4</v>
       </c>
       <c r="BP6" s="20">
-        <v>5.4011291152529202E-4</v>
+        <v>6.0805886155577298E-4</v>
       </c>
       <c r="BQ6" s="20">
-        <v>5.4025504650200918E-4</v>
+        <v>6.0821887704565604E-4</v>
       </c>
       <c r="BR6" s="20">
-        <v>5.4039721888266749E-4</v>
+        <v>6.0837893464487855E-4</v>
       </c>
       <c r="BS6" s="20">
-        <v>5.4053942867711023E-4</v>
+        <v>6.0853903436452193E-4</v>
       </c>
       <c r="BT6" s="20">
-        <v>5.4068167589518313E-4</v>
+        <v>6.086991762156704E-4</v>
       </c>
     </row>
     <row r="7" spans="1:72">
@@ -3138,185 +3158,185 @@
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="P7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="Q7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="R7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="S7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="T7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="U7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="V7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="W7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="X7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="Y7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="Z7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AA7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AB7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AC7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AD7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AE7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AF7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AG7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AH7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AI7" s="16">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AJ7" s="16">
-        <v>4.2033914976138416E-4</v>
-      </c>
-      <c r="AK7" s="24">
-        <v>4.2033914976138416E-4</v>
-      </c>
-      <c r="AL7" s="24">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
+      </c>
+      <c r="AK7" s="23">
+        <v>3.7161983445238052E-7</v>
+      </c>
+      <c r="AL7" s="23">
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AM7" s="25">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AN7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AO7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AP7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AQ7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AR7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AS7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AT7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AU7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AV7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AW7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AX7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AY7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="AZ7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BA7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BB7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BC7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BD7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BE7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BF7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BG7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BH7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BI7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BJ7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BK7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BL7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BM7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BN7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BO7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BP7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BQ7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BR7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BS7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="BT7" s="20">
-        <v>4.2033914976138416E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
     </row>
     <row r="8" spans="1:72">
-      <c r="A8" t="s">
+      <c r="A8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="13"/>
@@ -3417,10 +3437,10 @@
       <c r="AJ8" s="16">
         <v>2.8156039505680334E-3</v>
       </c>
-      <c r="AK8" s="24">
+      <c r="AK8" s="23">
         <v>2.8156039505680334E-3</v>
       </c>
-      <c r="AL8" s="24">
+      <c r="AL8" s="23">
         <v>2.8156039505680334E-3</v>
       </c>
       <c r="AM8" s="25">
@@ -3631,10 +3651,10 @@
       <c r="AJ9" s="16">
         <v>4.3071891857226225E-3</v>
       </c>
-      <c r="AK9" s="24">
+      <c r="AK9" s="23">
         <v>4.3071891857226225E-3</v>
       </c>
-      <c r="AL9" s="24">
+      <c r="AL9" s="23">
         <v>4.3071891857226225E-3</v>
       </c>
       <c r="AM9" s="25">
@@ -3741,10 +3761,10 @@
       </c>
     </row>
     <row r="10" spans="1:72">
-      <c r="A10" t="s">
+      <c r="A10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="13"/>
@@ -3843,10 +3863,10 @@
       <c r="AJ10" s="16">
         <v>2.3178432205516356E-4</v>
       </c>
-      <c r="AK10" s="24">
-        <v>2.3178432205516356E-4</v>
-      </c>
-      <c r="AL10" s="24">
+      <c r="AK10" s="23">
+        <v>2.3178432205516356E-4</v>
+      </c>
+      <c r="AL10" s="23">
         <v>2.3178432205516356E-4</v>
       </c>
       <c r="AM10" s="25">
@@ -4055,10 +4075,10 @@
       <c r="AJ11" s="16">
         <v>2.0246293667484216E-3</v>
       </c>
-      <c r="AK11" s="24">
-        <v>2.0246293667484216E-3</v>
-      </c>
-      <c r="AL11" s="24">
+      <c r="AK11" s="23">
+        <v>2.0246293667484216E-3</v>
+      </c>
+      <c r="AL11" s="23">
         <v>2.0246293667484216E-3</v>
       </c>
       <c r="AM11" s="25">
@@ -4165,10 +4185,10 @@
       </c>
     </row>
     <row r="12" spans="1:72">
-      <c r="A12" t="s">
+      <c r="A12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="13"/>
@@ -4235,10 +4255,10 @@
       <c r="AJ12" s="16">
         <v>5.9683256416215671E-4</v>
       </c>
-      <c r="AK12" s="24">
+      <c r="AK12" s="23">
         <v>5.9683256416215671E-4</v>
       </c>
-      <c r="AL12" s="24">
+      <c r="AL12" s="23">
         <v>5.9683256416215671E-4</v>
       </c>
       <c r="AM12" s="25">
@@ -4345,10 +4365,10 @@
       </c>
     </row>
     <row r="13" spans="1:72">
-      <c r="A13" s="8" t="s">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="17"/>
@@ -4419,10 +4439,10 @@
       <c r="AJ13" s="8">
         <v>0</v>
       </c>
-      <c r="AK13" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="24">
+      <c r="AK13" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="23">
         <v>0</v>
       </c>
       <c r="AM13" s="25">
@@ -4552,7 +4572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -5033,12 +5053,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.73046875" customWidth="1"/>
     <col min="3" max="3" width="18.265625" customWidth="1"/>
     <col min="4" max="5" width="16.73046875" customWidth="1"/>
@@ -5047,7 +5067,7 @@
     <col min="8" max="8" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="42.75">
+    <row r="1" spans="1:8" ht="28.5">
       <c r="A1" s="18" t="s">
         <v>57</v>
       </c>
@@ -5079,30 +5099,31 @@
       </c>
       <c r="B2" s="11">
         <f>$D2/(1-'Calculations Etc'!$B$2)*'Calibration Adjustments'!B19</f>
-        <v>8.3921322613283078E-4</v>
+        <v>1.2269199212468287E-3</v>
       </c>
       <c r="C2" s="11">
         <f>$D2*'Calibration Adjustments'!C19</f>
-        <v>2.6355456688469071E-4</v>
-      </c>
-      <c r="D2" s="11">
-        <v>2.6355456688469071E-4</v>
+        <v>3.8531369427586366E-4</v>
+      </c>
+      <c r="D2" s="26">
+        <f>'BHNVFEAL data'!AM2*'Calibration Adjustments'!D19</f>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="E2" s="11">
         <f>$D2*'Calibration Adjustments'!E19</f>
-        <v>2.6355456688469071E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="F2" s="11">
         <f>$D2/(1-'Calculations Etc'!$B$2)*'Calculations Etc'!$B$6+$D2*(1-'Calculations Etc'!$B$6)*'Calibration Adjustments'!F19</f>
-        <v>5.8016682947116776E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="G2" s="11">
         <f>$D2*'Calibration Adjustments'!G19</f>
-        <v>2.6355456688469071E-4</v>
+        <v>3.8531369427586366E-4</v>
       </c>
       <c r="H2" s="11">
         <f>D2*'Calculations Etc'!$B$11</f>
-        <v>6.5888641721172678E-4</v>
+        <v>9.6328423568965921E-4</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -5111,31 +5132,31 @@
       </c>
       <c r="B3" s="11">
         <f>$E3/(1-'Calculations Etc'!$B$3)*'Calibration Adjustments'!B20</f>
-        <v>5.6735511893623858E-3</v>
+        <v>5.6735511893623832E-3</v>
       </c>
       <c r="C3" s="11">
         <f>$E3*'Calibration Adjustments'!C20</f>
-        <v>1.7655503230029946E-3</v>
+        <v>1.7655503230029938E-3</v>
       </c>
       <c r="D3" s="11">
         <f>$E3*'Calibration Adjustments'!D20</f>
-        <v>1.7655503230029946E-3</v>
-      </c>
-      <c r="E3" s="11">
-        <f>AVERAGE('BHNVFEAL data'!P4:AL4)*'Calibration Adjustments'!E20</f>
-        <v>1.7655503230029946E-3</v>
+        <v>1.7655503230029938E-3</v>
+      </c>
+      <c r="E3" s="26">
+        <f>'BHNVFEAL data'!AM4*'Calibration Adjustments'!E20</f>
+        <v>1.7655503230029938E-3</v>
       </c>
       <c r="F3" s="11">
         <f>$E3/(1-'Calculations Etc'!$B$3)*'Calculations Etc'!$B$6+$E3*(1-'Calculations Etc'!$B$6)*'Calibration Adjustments'!F20</f>
-        <v>3.9149507995006596E-3</v>
+        <v>3.9149507995006579E-3</v>
       </c>
       <c r="G3" s="11">
         <f>$E3*'Calibration Adjustments'!G20</f>
-        <v>1.7655503230029946E-3</v>
+        <v>1.7655503230029938E-3</v>
       </c>
       <c r="H3" s="11">
         <f>D3*'Calculations Etc'!$B$11</f>
-        <v>4.4138758075074865E-3</v>
+        <v>4.4138758075074848E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -5151,9 +5172,9 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="16">
-        <f>AVERAGE('BHNVFEAL data'!O6:AL6)*'Calibration Adjustments'!E21</f>
-        <v>5.3600722376299567E-4</v>
+      <c r="E4" s="27">
+        <f>'BHNVFEAL data'!AM6*'Calibration Adjustments'!E21</f>
+        <v>6.0343668020558983E-4</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -5169,9 +5190,9 @@
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="16">
-        <f>AVERAGE('BHNVFEAL data'!E8:AL8)*'Calibration Adjustments'!E22</f>
-        <v>2.8156039505680313E-3</v>
+      <c r="B5" s="27">
+        <f>'BHNVFEAL data'!AM8*'Calibration Adjustments'!E22</f>
+        <v>2.8156039505680334E-3</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5225,23 +5246,23 @@
       </c>
       <c r="B7" s="11">
         <f>$D7/(1-'Calculations Etc'!$B$2)*'Calibration Adjustments'!B24</f>
-        <v>1.9004405332531825E-3</v>
+        <v>1.9004405332531829E-3</v>
       </c>
       <c r="C7" s="11">
         <f>$D7*'Calibration Adjustments'!C24</f>
-        <v>5.968325641621566E-4</v>
-      </c>
-      <c r="D7" s="11">
-        <f>AVERAGE('BHNVFEAL data'!V12:AL12)*'Calibration Adjustments'!D24</f>
-        <v>5.968325641621566E-4</v>
+        <v>5.9683256416215671E-4</v>
+      </c>
+      <c r="D7" s="26">
+        <f>'BHNVFEAL data'!AM12*'Calibration Adjustments'!D24</f>
+        <v>5.9683256416215671E-4</v>
       </c>
       <c r="E7" s="11">
         <f>$D7*'Calibration Adjustments'!E24</f>
-        <v>5.968325641621566E-4</v>
+        <v>5.9683256416215671E-4</v>
       </c>
       <c r="F7" s="11">
         <f>$D7/(1-'Calculations Etc'!$B$2)*'Calculations Etc'!$B$6+$D7*(1-'Calculations Etc'!$B$6)*'Calibration Adjustments'!F24</f>
-        <v>1.3138169471622208E-3</v>
+        <v>1.3138169471622213E-3</v>
       </c>
       <c r="G7" s="16">
         <f>AVERAGE('BHNVFEAL data'!AA12:AJ12)*'Calibration Adjustments'!G24</f>
@@ -5249,7 +5270,7 @@
       </c>
       <c r="H7" s="11">
         <f>D7*'Calculations Etc'!$B$11</f>
-        <v>1.4920814104053914E-3</v>
+        <v>1.4920814104053917E-3</v>
       </c>
     </row>
   </sheetData>
@@ -5264,8 +5285,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5316,8 +5337,8 @@
         <f>$D2*'Calibration Adjustments'!C28</f>
         <v>1.625585658993685E-4</v>
       </c>
-      <c r="D2" s="11">
-        <f>AVERAGE('BHNVFEAL data'!Y3:AL3)*'Calibration Adjustments'!D28</f>
+      <c r="D2" s="26">
+        <f>'BHNVFEAL data'!AM3*'Calibration Adjustments'!D28</f>
         <v>1.625585658993685E-4</v>
       </c>
       <c r="E2" s="11">
@@ -5343,31 +5364,31 @@
       </c>
       <c r="B3" s="11">
         <f>$E3/(1-'Calculations Etc'!$B$3)*'Calibration Adjustments'!B29</f>
-        <v>1.5166722171907963E-3</v>
+        <v>1.5166722171907955E-3</v>
       </c>
       <c r="C3" s="11">
         <f>$E3*'Calibration Adjustments'!C29</f>
-        <v>4.7197267347680614E-4</v>
+        <v>4.7197267347680587E-4</v>
       </c>
       <c r="D3" s="11">
         <f>$E3*'Calibration Adjustments'!D29</f>
-        <v>4.7197267347680614E-4</v>
-      </c>
-      <c r="E3" s="11">
-        <f>AVERAGE('BHNVFEAL data'!K5:AL5)*'Calibration Adjustments'!E29</f>
-        <v>4.7197267347680614E-4</v>
+        <v>4.7197267347680587E-4</v>
+      </c>
+      <c r="E3" s="26">
+        <f>'BHNVFEAL data'!AM5*'Calibration Adjustments'!E29</f>
+        <v>4.7197267347680587E-4</v>
       </c>
       <c r="F3" s="11">
         <f>$E3/(1-'Calculations Etc'!$B$3)*'Calculations Etc'!$B$6+$E3*(1-'Calculations Etc'!$B$6)*'Calibration Adjustments'!F29</f>
-        <v>1.0465574225195008E-3</v>
+        <v>1.0465574225195001E-3</v>
       </c>
       <c r="G3" s="11">
         <f>$E3*'Calibration Adjustments'!G29</f>
-        <v>4.7197267347680614E-4</v>
+        <v>4.7197267347680587E-4</v>
       </c>
       <c r="H3" s="11">
         <f>D3*'Calculations Etc'!$B$11</f>
-        <v>1.1799316836920153E-3</v>
+        <v>1.1799316836920146E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -5383,9 +5404,9 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="16">
-        <f>AVERAGE('BHNVFEAL data'!O6:AL6)*'Calibration Adjustments'!E30</f>
-        <v>5.3600722376299567E-4</v>
+      <c r="E4" s="29">
+        <f>'BHNVFEAL data'!AM7*'Calibration Adjustments'!E30</f>
+        <v>3.7161983445238052E-7</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -5396,7 +5417,7 @@
       </c>
       <c r="H4">
         <f>AVERAGE('BHNVFEAL data'!R7:AK7)*'Calibration Adjustments'!H30</f>
-        <v>4.2033914976138422E-4</v>
+        <v>3.7161983445238052E-7</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5405,7 +5426,7 @@
       </c>
       <c r="B5" s="16">
         <f>E5*'Calculations Etc'!B3</f>
-        <v>2.9668365557250754E-3</v>
+        <v>2.9668365557250762E-3</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5414,8 +5435,8 @@
         <v>0</v>
       </c>
       <c r="E5" s="16">
-        <f>AVERAGE('BHNVFEAL data'!E9:AL9)*'Calibration Adjustments'!E31</f>
-        <v>4.3071891857226216E-3</v>
+        <f>'BHNVFEAL data'!AM9*'Calibration Adjustments'!E31</f>
+        <v>4.3071891857226225E-3</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -5443,8 +5464,8 @@
         <v>0</v>
       </c>
       <c r="E6" s="16">
-        <f>AVERAGE('BHNVFEAL data'!F11:AL11)*'Calibration Adjustments'!E32</f>
-        <v>2.0246293667484229E-3</v>
+        <f>'BHNVFEAL data'!AM11*'Calibration Adjustments'!E32</f>
+        <v>2.0246293667484216E-3</v>
       </c>
       <c r="F6">
         <v>0</v>

</xml_diff>